<commit_message>
Add tweets related to the RUU TNI controversy, highlighting public sentiment and opposition
</commit_message>
<xml_diff>
--- a/Validasi Skripsi/chat_log.xlsx
+++ b/Validasi Skripsi/chat_log.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,79 +436,262 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Bagaimana tanggapan masyarakat terkait prabowo</t>
+          <t>Apakah RUU TNI baik bagi  Indonesia?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Based on the input text, it seems that the question is asking about the public's response or reaction to Prabowo, a former Indonesian military general and politician. Here's a possible answer:
-Tanggapan masyarakat terkait Prabowo sangat beragam dan terkadang kontroversial. Beberapa orang memandangnya sebagai seorang pemimpin yang berprinsip dan memiliki visi jangka panjang untuk meningkatkan kesejahteraan rakyat, sementara lainnya memandangnya sebagai seorang yang korup dan tidak memiliki integritas.
-Beberapa faktor yang mempengaruhi tanggapan masyarakat terhadap Prabowo antara lain adalah:
-1. Sejarah politik Prabowo: Prabowo memiliki sejarah politik yang panjang dan kompleks, termasuk pernah menjadi Wakil Presiden Indonesia dan calon Presiden beberapa kali. Hal ini mempengaruhi pandangan masyarakat tentang dirinya.
-2. Keterlibatan dalam kasus 1998: Prabowo pernah terlibat dalam kasus 1998, yang melibatkan penghilangan paksa beberapa ribu orang, termasuk beberapa orang yang menjadi korban. Hal ini mempengaruhi pandangan masyarakat tentang dirinya.
-3. Keterlibatan dalam korupsi: Prabowo pernah terlibat dalam beberapa kasus korupsi, termasuk kasus penggelapan dana APBN. Hal ini mempengaruhi pandangan masyarakat tentang dirinya.
-4. Keterlibatan dalam konf</t>
+          <t>Berdasarkan informasi yang tersedia, RUU TNI (Rancangan Undang-Undang Tentara Nasional Indonesia) memiliki beberapa aspek yang dapat dipertimbangkan baik bagi Indonesia. Berikut beberapa poin penting:
+1. **Penguatan Kemampuan TNI**: RUU TNI dapat meningkatkan kemampuan TNI dalam menjaga keamanan dan stabilitas nasional. Dengan demikian, Indonesia dapat lebih siap menghadapi ancaman keamanan dari dalam dan luar negeri.
+2. **Peningkatan Profesionalisme TNI**: RUU TNI dapat meningkatkan profesionalisme TNI dengan mengatur standar pelatihan, pengembangan karier, dan sistem penghargaan yang lebih baik. Hal ini dapat meningkatkan kualitas dan kemampuan TNI dalam menjalankan tugasnya.
+3. **Pengawasan dan Akuntabilitas TNI**: RUU TNI dapat meningkatkan pengawasan dan akuntabilitas TNI dengan mengatur sistem pengawasan yang lebih efektif dan transparan. Hal ini dapat meningkatkan kepercayaan masyarakat terhadap TNI dan mengurangi kemungkinan pelanggaran hak asasi manusia.
+4. **Pengintegrasian TNI dengan Masyarakat**: RUU TNI dapat meningkatkan pengintegrasian TNI dengan masyarakat dengan mengatur program-program yang dapat meningkatkan interaksi dan komunikasi antara TNI dan masyarakat. Hal ini dapat meningkatkan kepercayaan masyarakat terhadap TNI dan mengurangi kemungkinan konflik.
+Namun, perlu diingat bahwa RUU TNI juga memiliki beberapa kelemahan dan kritik. Oleh karena itu, perlu dilakukan diskusi dan debat yang lebih lanjut untuk memastikan bahwa RUU TNI dapat membawa manfaat bagi Indonesia dan masyarakatnya.
+Dalam keseluruhan, RUU TNI dapat menjadi baik bagi Indonesia jika dapat meningkatkan kemampuan, profesionalisme, dan akuntabilitas TNI, serta mengintegrasikan TNI dengan masyarakat. Namun, perlu diingat bahwa RUU TNI juga perlu diawasi dan dikritik untuk memastikan bahwa tidak ada pelanggaran hak asasi manusia dan kepentingan masyarakat.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Jika Prabowo adalah pelanggar HAM apakah kejadian tersebut akan terulang selama ia menjabat menjadi presiden?</t>
+          <t>Bagaimana tanggapan masyarakat terkait RUU TNI</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Berdasarkan informasi yang tersedia, tidak ada bukti yang kuat bahwa Prabowo Subianto adalah pelanggar HAM. Namun, terdapat beberapa kontroversi dan kritik yang diajukan terhadapnya terkait dengan pelanggaran HAM di masa lalu.
-Sebagai presiden, Prabowo Subianto memiliki kewajiban untuk menjaga dan menghormati hak asasi manusia (HAM) di Indonesia. Jika ia terbukti melakukan pelanggaran HAM selama menjabat sebagai presiden, maka itu akan menjadi masalah yang serius dan dapat mempengaruhi kepercayaan masyarakat terhadap pemerintahan.
-Namun, perlu diingat bahwa presiden memiliki kewajiban untuk menjalankan tugasnya dengan baik dan menghormati konstitusi dan hukum yang berlaku di Indonesia. Jika terdapat bukti yang kuat bahwa Prabowo Subianto melakukan pelanggaran HAM, maka itu akan menjadi masalah yang serius dan dapat diproses secara hukum.
-Dalam menjalankan tugasnya, presiden harus memastikan bahwa semua kebijakan dan tindakan yang diambil tidak melanggar HAM dan tidak membahayakan masyarakat. Oleh karena itu, penting bagi masyarakat untuk terus memantau dan mengawasi kinerja presiden dan pemerintahan dalam menjaga dan menghormati HAM.</t>
+          <t>Berdasarkan informasi yang tersedia, tanggapan masyarakat terkait RUU TNI dapat disimpulkan sebagai berikut:
+1. Masyarakat menolak RUU TNI karena dianggap dapat membahayakan keamanan dan kesejahteraan masyarakat.
+2. Masyarakat khawatir bahwa RUU TNI dapat memberikan kekuasaan yang terlalu besar kepada TNI dan dapat mengancam demokrasi dan hak asasi manusia.
+3. Masyarakat juga mengkritik RUU TNI karena dianggap tidak transparan dan tidak melibatkan masyarakat dalam proses pengambilan keputusan.
+4. Beberapa masyarakat juga menganggap bahwa RUU TNI dapat membantu meningkatkan kemampuan TNI dalam menjaga keamanan dan stabilitas nasional.
+5. Namun, masih banyak masyarakat yang belum memahami isi dan tujuan RUU TNI sehingga perlu dilakukan sosialisasi dan edukasi yang lebih baik.
+Dalam keseluruhan, tanggapan masyarakat terkait RUU TNI sangat beragam dan perlu dilakukan dialog yang lebih konstruktif dan transparan untuk memahami kebutuhan dan kekhawatiran masyarakat.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Siapa itu prabowo?</t>
+          <t>Apa yang menjadi kekhawatiran masyarakat terkait RUU TNI?</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Berdasarkan informasi yang tersedia, Prabowo adalah seorang tokoh politik dan militer Indonesia. Ia pernah menjabat sebagai Panglima Komando Pasukan Khusus (Kopassus) dan juga pernah menjadi calon presiden dalam beberapa kali pemilihan umum di Indonesia.</t>
+          <t>Berdasarkan informasi yang tersedia, kekhawatiran masyarakat terkait RUU TNI adalah sebagai berikut:
+1. Kekhawatiran tentang keterlibatan TNI dalam politik dan pengaruhnya terhadap demokrasi.
+2. Kekhawatiran tentang penambahan kewenangan TNI dan implikasinya terhadap hak asasi manusia.
+3. Kekhawatiran tentang penggunaan kekuatan militer untuk menyelesaikan konflik dan implikasinya terhadap korban sipil.
+4. Kekhawatiran tentang keterlibatan TNI dalam bisnis dan korupsi.
+5. Kekhawatiran tentang keterbatasan transparansi dan akuntabilitas TNI dalam penggunaan anggaran dan sumber daya.
+6. Kekhawatiran tentang keterlibatan TNI dalam penyelesaian konflik horizontal dan implikasinya terhadap keamanan nasional.
+7. Kekhawatiran tentang keterbatasan peran TNI dalam menjaga keamanan nasional dan implikasinya terhadap ketergantungan pada kekuatan asing.
+Dalam keseluruhan, kekhawatiran masyarakat terkait RUU TNI berkaitan dengan keterlibatan TNI dalam politik, kewenangan, dan penggunaan kekuatan militer, serta implikasinya terhadap demokrasi, hak asasi manusia, dan keamanan nasional.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Apa latar belakang dan profil Prabowo Subianto?</t>
+          <t>Bagaimana dampak RUU TNI terhadap demokrasi dan hak asasi manusia?</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Latar belakang dan profil Prabowo Subianto:
-Prabowo Subianto adalah seorang politikus dan mantan jenderal Tentara Nasional Indonesia (TNI) yang lahir pada tanggal 17 Oktober 1951 di Jakarta, Indonesia. Ia adalah putra dari Sumitro Djojohadikusumo, seorang ekonom dan politikus Indonesia yang terkemuka.
-Prabowo memulai karier militernya pada tahun 1974 dan dengan cepat naik pangkat menjadi jenderal. Ia pernah menjabat sebagai Panglima Komando Pasukan Khusus (Kopassus) dan Panglima Tentara Nasional Indonesia (TNI) Angkatan Darat.
-Pada tahun 1998, Prabowo terlibat dalam krisis politik yang menyebabkan Presiden Soeharto mengundurkan diri. Ia kemudian dipecat dari jabatan militernya dan meninggalkan Indonesia. Setelah itu, ia tinggal di Yordania dan kemudian kembali ke Indonesia pada tahun 2008.
-Pada tahun 2014, Prabowo memutuskan untuk terjun ke dunia politik dan menjadi calon presiden dalam Pemilihan Umum Presiden Indonesia 2014. Ia kalah dalam pemilihan tersebut, tetapi tetap menjadi figur politik yang penting di Indonesia.
-Pada tahun 2018, Prabowo kembali menjadi calon presiden dalam Pemilihan Umum Presiden Indonesia 2019 dan kalah lagi dalam pemilihan tersebut. Meskipun demikian, ia tetap menjadi figur politik yang berpengaruh di Indonesia dan terus aktif dalam kegiatan politik.
-Dalam profilnya, Prabowo dikenal sebagai seorang yang memiliki kemampuan kepemimpinan yang kuat dan memiliki visi yang jelas untuk membangun Indonesia. Ia juga dikenal sebagai seorang yang memiliki kemampuan komunikasi yang baik dan dapat berbicara dengan berbagai kalangan masyarakat.</t>
+          <t>Dampak RUU TNI terhadap demokrasi dan hak asasi manusia dapat berupa:
+1. Pengurangan kebebasan sipil: RUU TNI dapat memberikan kekuasaan yang lebih besar kepada militer, sehingga dapat mengurangi kebebasan sipil dan hak asasi manusia.
+2. Penggunaan kekerasan: RUU TNI dapat memungkinkan penggunaan kekerasan oleh militer dalam menangani konflik dan gangguan keamanan, yang dapat berdampak pada pelanggaran hak asasi manusia.
+3. Pengurangan transparansi dan akuntabilitas: RUU TNI dapat membuat militer menjadi lebih tidak transparan dan tidak akuntabel, sehingga dapat menghambat proses demokrasi dan pengawasan terhadap kekuasaan.
+4. Pengaruh pada stabilitas politik: RUU TNI dapat membuat stabilitas politik menjadi tidak stabil, karena dapat memungkinkan militer untuk campur tangan dalam urusan politik dan mengganggu proses demokrasi.
+5. Pelanggaran hak asasi manusia: RUU TNI dapat memungkinkan pelanggaran hak asasi manusia, seperti hak atas kebebasan berbicara, hak atas kebebasan bergerak, dan hak atas keamanan pribadi.
+6. Pengurangan peran sipil dalam pengambilan keputusan: RUU TNI dapat membuat peran sipil dalam pengambilan keputusan menjadi lebih kecil, sehingga dapat menghambat proses demokrasi dan pengawasan terhadap kekuasaan.
+Dalam keseluruhan, RUU TNI dapat berdampak negatif terhadap demokrasi dan hak asasi manusia, karena dapat membuat militer menjadi lebih dominan dan mengurangi peran sipil dalam pengambilan keputusan. Oleh karena itu, perlu dilakukan pengawasan yang ketat terhadap RUU TNI dan memastikan bahwa hak asasi manusia dan demokrasi tetap terjaga.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Apa pengalaman politik Prabowo Subianto?</t>
+          <t>Apa potensi pelanggaran hak asasi manusia yang dapat terjadi akibat RUU TNI?</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Berdasarkan informasi yang tersedia, pengalaman politik Prabowo Subianto dapat dijelaskan sebagai berikut:
-Prabowo Subianto memiliki pengalaman politik yang luas dan panjang. Ia pernah menjabat sebagai Panglima Komando Strategis Angkatan Darat (Kostrad) dan Panglima Komando Pasukan Khusus (Kopassus). Ia juga pernah menjabat sebagai Menteri Pertahanan dan Keamanan pada tahun 2000-2001.
-Pada tahun 2004, Prabowo Subianto mendirikan Partai Gerakan Indonesia Raya (Gerindra) dan menjadi ketua umum partai tersebut. Ia juga pernah menjadi calon presiden pada Pemilihan Umum Presiden Indonesia tahun 2014 dan 2019.
-Selain itu, Prabowo Subianto juga memiliki pengalaman dalam bidang politik internasional. Ia pernah menjabat sebagai Duta Besar Indonesia untuk Jordan dan Palestina pada tahun 2005-2009.
-Dalam karier politiknya, Prabowo Subianto dikenal sebagai seorang politikus yang memiliki visi dan misi yang kuat untuk membangun Indonesia. Ia juga dikenal sebagai seorang yang memiliki kemampuan leadership yang baik dan mampu menginspirasi orang lain.</t>
+          <t>Berdasarkan informasi yang tersedia, potensi pelanggaran hak asasi manusia yang dapat terjadi akibat RUU TNI adalah sebagai berikut:
+1. Pelanggaran hak kebebasan berbicara dan berekspresi, karena RUU TNI dapat membatasi kebebasan berbicara dan berekspresi masyarakat, terutama bagi mereka yang memiliki pandangan yang berbeda dengan pemerintah.
+2. Pelanggaran hak atas keamanan dan perlindungan, karena RUU TNI dapat memberikan kewenangan yang terlalu luas kepada TNI untuk melakukan tindakan yang dapat membahayakan keselamatan masyarakat.
+3. Pelanggaran hak atas keadilan dan perlindungan hukum, karena RUU TNI dapat membatasi akses masyarakat terhadap keadilan dan perlindungan hukum, terutama bagi mereka yang menjadi korban pelanggaran hak asasi manusia.
+4. Pelanggaran hak atas kebebasan bergerak dan berkumpul, karena RUU TNI dapat membatasi kebebasan bergerak dan berkumpul masyarakat, terutama bagi mereka yang ingin melakukan demonstrasi atau unjuk rasa.
+5. Pelanggaran hak atas kehidupan yang layak, karena RUU TNI dapat membahayakan keselamatan dan kesejahteraan masyarakat, terutama bagi mereka yang tinggal di daerah konflik.
+6. Pelanggaran hak atas perlindungan anak dan perempuan, karena RUU TNI dapat membahayakan keselamatan dan kesejahteraan anak dan perempuan, terutama bagi mereka yang tinggal di daerah konflik.
+Dalam hal ini, penting bagi masyarakat untuk memantau dan mengkritisi RUU TNI agar tidak membahayakan hak asasi manusia.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Jadi RUU TNI sebaiknya ditolak?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Berdasarkan informasi yang tersedia, tidak dapat disimpulkan bahwa RUU TNI harus ditolak. Namun, beberapa poin penting perlu diperhatikan.
+Pertama, RUU TNI dibahas dan disahkan melalui mekanisme resmi yang sah dan terbuka (Informasi 4). Hal ini menunjukkan bahwa proses pengesahan RUU TNI telah memenuhi prosedur yang benar.
+Kedua, RUU TNI bertujuan untuk mereformasi sektor pertahanan agar TNI dapat berperan lebih adaptif sesuai kebutuhan zaman, tetap profesional, dan tunduk pada supremasi sipil (Informasi 4). Hal ini dapat dipahami sebagai upaya untuk meningkatkan profesionalisme dan akuntabilitas TNI.
+Namun, beberapa pihak juga mengkritik RUU TNI karena khawatir akan membuka peluang bagi TNI untuk terlibat dalam politik praktis dan mengancam supremasi sipil (Informasi 5, 6, dan 7). Mereka juga khawatir bahwa RUU TNI dapat membuka jalan bagi TNI untuk menguasai jabatan sipil dan mengancam demokrasi.
+Oleh karena itu, penting bagi masyarakat untuk tetap kritis dan memantau perkembangan RUU TNI agar tidak disalahgunakan untuk kepentingan politik atau mengancam supremasi sipil. Namun, tidak dapat disimpulkan bahwa RUU TNI harus ditolak secara mutlak. Perlu adanya diskusi yang lebih lanjut dan transparan tentang isi dan tujuan RUU TNI.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Bagaimana RUU TNI dapat mempengaruhi supremasi sipil di Indonesia?</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Berdasarkan informasi yang tersedia, RUU TNI dapat mempengaruhi supremasi sipil di Indonesia dalam beberapa cara:
+Pertama, beberapa pihak khawatir bahwa RUU TNI akan mengembalikan dwifungsi ABRI, di mana militer akan memiliki peran yang lebih besar dalam pemerintahan sipil. Hal ini dapat mengancam supremasi sipil dan mengurangi peran warga negara dalam pengambilan keputusan.
+Namun, beberapa informasi lainnya menyatakan bahwa RUU TNI justru akan memperkuat profesionalitas TNI dan mengedepankan supremasi sipil. Peran TNI dalam jabatan sipil akan diatur dan diawasi secara ketat, sehingga tidak akan mengancam supremasi sipil.
+Informasi lainnya juga menyatakan bahwa RUU TNI diperlukan untuk melindungi Indonesia dari ancaman siber dan untuk memperkuat kemampuan TNI dalam menjaga keamanan negara.
+Namun, beberapa pihak juga khawatir bahwa RUU TNI dapat membuka peluang bagi militer untuk memiliki peran yang lebih besar dalam pemerintahan sipil, sehingga dapat mengancam supremasi sipil.
+Dalam keseluruhan, RUU TNI dapat mempengaruhi supremasi sipil di Indonesia, baik positif maupun negatif, tergantung pada bagaimana RUU tersebut diimplementasikan dan diawasi. Oleh karena itu, perlu adanya diskusi yang lebih lanjut dan transparansi dalam proses pengambilan keputusan terkait RUU TNI.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Bagaimana RUU TNI dapat mempengaruhi hak asasi manusia di Indonesia?</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>RUU TNI dapat mempengaruhi hak asasi manusia di Indonesia dengan beberapa cara. Pertama, jika RUU TNI disahkan, maka peran TNI dalam jabatan sipil akan diatur dan diawasi secara ketat. Namun, jika tidak diawasi dengan baik, maka dapat terjadi pelanggaran hak asasi manusia, seperti penggunaan kekuasaan atas senjata untuk mengintimidasi atau menindas warga sipil.
+Kedua, jika TNI diberikan kekuasaan yang lebih besar dalam jabatan sipil, maka dapat terjadi penggunaan kekuasaan yang tidak proporsional dan dapat mengancam hak-hak dasar warga sipil, seperti hak kebebasan berbicara, hak berkumpul, dan hak berorganisasi.
+Ketiga, RUU TNI juga dapat mempengaruhi hak asasi manusia dengan cara menguatkan peran TNI dalam menghadapi ancaman siber. Jika tidak diawasi dengan baik, maka dapat terjadi penggunaan teknologi untuk mengintimidasi atau mengawasi warga sipil secara tidak proporsional.
+Namun, perlu diingat bahwa RUU TNI juga dapat mempengaruhi hak asasi manusia dengan cara positif, seperti meningkatkan profesionalitas TNI dan menguatkan supremasi sipil. Oleh karena itu, penting untuk memastikan bahwa RUU TNI diawasi dan diatur dengan baik agar tidak terjadi pelanggaran hak asasi manusia.
+Dalam konteks ini, penting untuk memastikan bahwa RUU TNI tidak mengancam hak asasi manusia dan bahwa TNI tetap berfungsi sebagai institusi yang profesional dan demokratis. Oleh karena itu, perlu adanya pengawasan yang ketat dan transparan terhadap implementasi RUU TNI agar tidak terjadi pelanggaran hak asasi manusia.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Apa yang dapat terjadi jika TNI diberikan kekuasaan yang lebih besar dalam jabatan sipil?</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Jika TNI diberikan kekuasaan yang lebih besar dalam jabatan sipil, maka beberapa hal buruk dapat terjadi. Pertama, demokrasi dan supremasi sipil dapat terancam karena kekuasaan militer akan meningkatkan pengaruhnya dalam pemerintahan sipil. Kedua, jabatan pemerintahan akan diisi oleh orang-orang yang tidak memiliki kompetensi dan inteligensi yang cukup, tetapi memiliki kekuasaan atas senjata. Hal ini dapat menyebabkan kebijakan yang tidak berpihak pada rakyat dan hanya melayani kepentingan militer.
+Ketiga, RUU TNI dapat membuka peluang bagi militer untuk ikut campur dalam politik praktis dan pemilu tanpa harus mengundurkan diri. Keempat, korupsi dan kezaliman dapat meningkat karena militer akan memiliki kekuasaan yang lebih besar dalam pemerintahan. Kelima, rakyat akan kehilangan hak-haknya dan nyawanya akan terancam karena militer akan memiliki kekuasaan yang lebih besar dalam mengatur kehidupan masyarakat.
+Dalam jangka panjang, hal ini dapat menyebabkan demokrasi dan reformasi yang telah dicapai selama ini menjadi sia-sia. Oleh karena itu, penting bagi masyarakat untuk tetap kritis dan menolak RUU TNI yang dapat membahayakan demokrasi dan kehidupan masyarakat.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Berikan saya alasan mengapa harus menolak RUU TNI</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Berdasarkan informasi yang tersedia, berikut adalah beberapa alasan mengapa harus menolak RUU TNI:
+1. RUU TNI dapat mengancam supremasi sipil karena memberikan peran yang terlalu besar kepada TNI dalam jabatan sipil, sehingga dapat mengganggu keseimbangan kekuasaan dalam negara.
+2. RUU TNI dapat membuka peluang bagi militer untuk mengintervensi kekuasaan sipil dan mengancam kebebasan sipil.
+3. Pengesahan RUU TNI dapat dianggap sebagai upaya untuk melindungi kepentingan politik tertentu, seperti melindungi Prabowo Subianto dari kudeta.
+4. RUU TNI dapat mengganggu keseimbangan kekuasaan dalam negara dan membuka peluang bagi militer untuk menguasai kekuasaan sipil.
+5. YLBHI menilai RUU TNI inkonstitusional dan dapat mengancam kebebasan sipil, sehingga harus ditolak.
+Dengan demikian, RUU TNI harus ditolak karena dapat mengancam supremasi sipil, kebebasan sipil, dan keseimbangan kekuasaan dalam negara.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Apakah RUU TNI buruk bagi Indonesia?</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Berdasarkan informasi yang tersedia, tidak dapat disimpulkan bahwa RUU TNI buruk bagi Indonesia. Ada beberapa informasi yang mendukung RUU TNI, seperti Informasi 1, 3, 4, dan 10, yang menyatakan bahwa RUU TNI adalah bagian dari upaya reformasi sektor pertahanan untuk membuat TNI lebih adaptif, profesional, dan tunduk pada supremasi sipil.
+Namun, ada juga beberapa informasi yang menolak RUU TNI, seperti Informasi 2, 5, 6, 7, 8, dan 9, yang menyatakan bahwa RUU TNI dapat membahayakan demokrasi dan supremasi sipil, serta dapat memperkuat dwifungsi TNI.
+Dalam hal ini, perlu diingat bahwa RUU TNI telah disahkan dan menjadi Undang-Undang. Oleh karena itu, perlu diadakan diskusi dan debat yang konstruktif untuk memahami isi dan implikasi dari RUU TNI, serta untuk memastikan bahwa RUU TNI dapat dijalankan dengan baik dan tidak membahayakan demokrasi dan supremasi sipil.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Apa yang menjadi pertimbangan utama dalam menilai RUU TNI sebagai baik atau buruk bagi Indonesia?</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Pertimbangan utama dalam menilai RUU TNI sebagai baik atau buruk bagi Indonesia adalah memahami isi dan tujuan revisi UU TNI secara objektif dan tidak terpengaruh oleh hoaks atau provokasi. Beberapa hal yang perlu dipertimbangkan adalah:
+1. Apakah RUU TNI tetap mengedepankan supremasi sipil dan mengatur peran TNI dalam jabatan sipil secara ketat?
+2. Apakah RUU TNI dapat memperkuat profesionalitas TNI dan meningkatkan kemampuan pertahanan nasional?
+3. Apakah proses pembahasan dan pengesahan RUU TNI dilakukan melalui mekanisme resmi yang sah dan terbuka?
+4. Apakah RUU TNI dapat membantu meningkatkan kesejahteraan dan keamanan rakyat Indonesia?
+Dengan mempertimbangkan hal-hal tersebut, maka kita dapat menilai RUU TNI secara objektif dan membuat keputusan yang bijak bagi kepentingan Indonesia.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Jadi RUU TNI itu buruk bagi Indonesia?</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Tidak, tidak semua informasi mengatakan bahwa RUU TNI itu buruk bagi Indonesia. Beberapa informasi justru mengatakan bahwa RUU TNI itu bagus dan perlu didukung karena dapat memperkuat profesionalitas TNI, menjaga supremasi sipil, dan membantu menjaga keamanan Indonesia. Hanya beberapa informasi yang mengkritik RUU TNI dan mengatakan bahwa itu dapat membahayakan demokrasi dan supremasi sipil. Oleh karena itu, perlu diwaspadai hoaks dan provokasi yang dapat mempengaruhi opini publik.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Jadi RUU TNI itu buruk bagi Indonesia?</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Tidak dapat disimpulkan bahwa RUU TNI itu buruk bagi Indonesia. Informasi yang tersedia menunjukkan adanya perbedaan pendapat dan persepsi tentang RUU TNI.
+Beberapa informasi seperti Informasi 1, 4, 6, dan 7 menunjukkan bahwa RUU TNI bertujuan untuk meningkatkan profesionalitas TNI, mengedepankan supremasi sipil, dan memperkuat peran TNI dalam menjaga keamanan dan stabilitas nasional. Informasi 9 juga menunjukkan bahwa RUU TNI telah disetujui oleh seluruh fraksi DPR.
+Namun, informasi lain seperti Informasi 3, 5, 8, dan 10 menunjukkan adanya kekhawatiran dan kritik terhadap RUU TNI, seperti kemungkinan penggunaan kekuasaan militer untuk mengintimidasi rakyat, mengembalikan dwifungsi ABRI, dan melindungi kepentingan individu.
+Dalam keseluruhan, perlu diadakan diskusi dan analisis yang lebih lanjut untuk memahami isi dan dampak RUU TNI terhadap Indonesia.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Bagaimana tanggapan masyarakat terhadap RUU TNII?</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Berdasarkan informasi yang tersedia, tanggapan masyarakat terhadap RUU TNI sangat beragam. Ada yang mendukung dan ada yang menolak.
+Sebagian masyarakat mendukung RUU TNI karena mereka percaya bahwa RUU ini akan membantu meningkatkan kemampuan dan profesionalisme TNI, serta membuat TNI lebih adaptif dan sesuai dengan kebutuhan zaman. Mereka juga percaya bahwa RUU ini akan membantu meningkatkan supremasi sipil dan mengurangi keterlibatan TNI dalam politik praktis.
+Namun, sebagian lainnya menolak RUU TNI karena mereka khawatir bahwa RUU ini akan memberikan kekuasaan yang terlalu besar kepada TNI dan mengancam supremasi sipil. Mereka juga khawatir bahwa RUU ini akan membuka peluang bagi TNI untuk ikut serta dalam pemilu dan politik praktis tanpa harus mengundurkan diri.
+Ada juga yang mengkritik RUU TNI karena mereka percaya bahwa RUU ini hanya untuk melindungi kepentingan tertentu, seperti Prabowo Subianto, dan bukan untuk kepentingan rakyat. Mereka juga mengkritik bahwa RUU ini tidak transparan dan tidak melibatkan masyarakat dalam proses pengambilan keputusan.
+Dalam beberapa informasi, terlihat bahwa masyarakat juga khawatir tentang kemungkinan TNI akan menjadi lebih dominan dalam pemerintahan dan mengancam demokrasi. Mereka juga mengkritik bahwa RUU ini tidak sesuai dengan prinsip demokrasi dan supremasi sipil.
+Dalam keseluruhan, tanggapan masyarakat terhadap RUU TNI sangat beragam dan terpolarisasi. Ada yang mendukung dan ada yang menolak, dan masing-masing memiliki alasan dan kekhawatiran yang berbeda-beda.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Mengapa masyarakat khawatir tentang kemungkinan TNI akan menjadi lebih dominan dalam pemerintahan?</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Masyarakat khawatir tentang kemungkinan TNI akan menjadi lebih dominan dalam pemerintahan karena beberapa alasan. Pertama, RUU TNI ini dianggap sebagai upaya untuk mengembalikan dwifungsi ABRI yang pernah ada pada masa pemerintahan Soeharto, di mana TNI memiliki peran yang sangat besar dalam pemerintahan dan politik. Kedua, masyarakat khawatir bahwa dengan disahkannya RUU TNI, TNI akan menjadi lebih kuat dan dominan dalam pemerintahan, sehingga dapat mengancam supremasi sipil dan demokrasi. Ketiga, beberapa pihak juga khawatir bahwa RUU TNI ini akan memperkuat kekuasaan militer dan mengurangi peran sipil dalam pemerintahan. Oleh karena itu, masyarakat khawatir bahwa RUU TNI ini akan membawa Indonesia kembali ke masa lalu yang otoriter dan tidak demokratis.</t>
         </is>
       </c>
     </row>

</xml_diff>